<commit_message>
turned u into un.
</commit_message>
<xml_diff>
--- a/List_SpanishMorphemes.xlsx
+++ b/List_SpanishMorphemes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bensteinberg/Desktop/Home/UCLA Linguistics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bensteinberg/Desktop/Home/UCLA Linguistics/spanish-morpheme/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F481F186-D9A1-4F47-90B4-BD4521F9E051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C95A2F8C-4E64-784B-B386-DA934727942B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25200" windowHeight="15320" xr2:uid="{BB6888A7-CFF3-47A6-A7B0-8D725AB4101D}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="500" windowWidth="25200" windowHeight="15320" xr2:uid="{BB6888A7-CFF3-47A6-A7B0-8D725AB4101D}"/>
   </bookViews>
   <sheets>
     <sheet name="List of Spanish Morphemes" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -580,10 +580,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -904,15 +901,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BB13061-DE0E-4CBC-847F-B92815CE8E81}">
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:J70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -932,67 +929,79 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
+      <c r="J2" s="10"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="C3" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="10" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1012,14 +1021,14 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
@@ -1039,15 +1048,14 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="16"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>20</v>
       </c>
@@ -1067,7 +1075,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
@@ -1087,14 +1095,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -1114,18 +1122,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="B13" s="16"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>32</v>
       </c>
@@ -1145,7 +1152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>32</v>
       </c>
@@ -1196,9 +1203,8 @@
       <c r="A19" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B19" s="16"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
@@ -1256,16 +1262,16 @@
       <c r="A26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27" s="20" t="s">
+      <c r="A27" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B27" s="21" t="s">
+      <c r="B27" s="18" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="D27" s="23" t="s">
+      <c r="C27" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="20" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1396,55 +1402,51 @@
       <c r="A41" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="16"/>
-      <c r="C41" s="17"/>
-      <c r="D41" s="17"/>
+      <c r="C41" s="16"/>
+      <c r="D41" s="16"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A42" s="18"/>
-      <c r="B42" s="16"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B43" s="16" t="s">
+      <c r="B43" t="s">
         <v>112</v>
       </c>
-      <c r="C43" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="16" t="s">
+      <c r="C43" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B44" s="16" t="s">
+      <c r="B44" t="s">
         <v>113</v>
       </c>
-      <c r="C44" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D44" s="16" t="s">
+      <c r="C44" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="18" t="s">
+      <c r="A45" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B45" s="16" t="s">
+      <c r="B45" t="s">
         <v>113</v>
       </c>
-      <c r="C45" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D45" s="16" t="s">
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1452,9 +1454,8 @@
       <c r="A46" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="17"/>
+      <c r="C46" s="16"/>
+      <c r="D46" s="16"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="1"/>
@@ -1715,7 +1716,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="5" t="s">
         <v>132</v>
       </c>
       <c r="C67" t="s">

</xml_diff>